<commit_message>
NextYear dataset without Msk&Spb
</commit_message>
<xml_diff>
--- a/migforecasting/underground/test-2.xlsx
+++ b/migforecasting/underground/test-2.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Тест прогнозов this-next" sheetId="1" r:id="rId1"/>
+    <sheet name="this-next (без Мск и Спб)" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="14">
   <si>
     <t>train (MAPE)</t>
   </si>
@@ -55,6 +56,12 @@
   </si>
   <si>
     <t>NN (64,64,64,64,1) (citiesdataset-1.csv)</t>
+  </si>
+  <si>
+    <t>Random Forest-100 (citiesdataset-2.csv) - this year</t>
+  </si>
+  <si>
+    <t>Random Forest-100 (citiesdataset-NY-2.csv) - next year</t>
   </si>
 </sst>
 </file>
@@ -224,6 +231,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -344,6 +352,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -486,6 +495,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1411,8 +1421,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:T59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U28" sqref="U28"/>
+    <sheetView topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3:J57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3100,4 +3110,799 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C3:J57"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="12" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" customWidth="1"/>
+    <col min="9" max="9" width="14.7109375" customWidth="1"/>
+    <col min="10" max="10" width="13.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="1"/>
+      <c r="H3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J3" s="1"/>
+    </row>
+    <row r="4" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C4" s="2"/>
+      <c r="D4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C5" s="2">
+        <v>1</v>
+      </c>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="H5" s="2">
+        <v>1</v>
+      </c>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+    </row>
+    <row r="6" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C6" s="2">
+        <f>C5+1</f>
+        <v>2</v>
+      </c>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="H6" s="2">
+        <f>H5+1</f>
+        <v>2</v>
+      </c>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+    </row>
+    <row r="7" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C7" s="2">
+        <f t="shared" ref="C7:C54" si="0">C6+1</f>
+        <v>3</v>
+      </c>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="H7" s="2">
+        <f t="shared" ref="H7:H54" si="1">H6+1</f>
+        <v>3</v>
+      </c>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+    </row>
+    <row r="8" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C8" s="2">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="H8" s="2">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+    </row>
+    <row r="9" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C9" s="2">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="H9" s="2">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+    </row>
+    <row r="10" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C10" s="2">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="H10" s="2">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+    </row>
+    <row r="11" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C11" s="2">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="H11" s="2">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+    </row>
+    <row r="12" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C12" s="2">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="H12" s="2">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+    </row>
+    <row r="13" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C13" s="2">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="H13" s="2">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+    </row>
+    <row r="14" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C14" s="2">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="H14" s="2">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+    </row>
+    <row r="15" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C15" s="2">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="H15" s="2">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+    </row>
+    <row r="16" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C16" s="2">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="H16" s="2">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+    </row>
+    <row r="17" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C17" s="2">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="H17" s="2">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+    </row>
+    <row r="18" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C18" s="2">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="H18" s="2">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+    </row>
+    <row r="19" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C19" s="2">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="H19" s="2">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+    </row>
+    <row r="20" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C20" s="2">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="H20" s="2">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
+    </row>
+    <row r="21" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C21" s="2">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="H21" s="2">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
+    </row>
+    <row r="22" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C22" s="2">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="H22" s="2">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
+    </row>
+    <row r="23" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C23" s="2">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="H23" s="2">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
+    </row>
+    <row r="24" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C24" s="2">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="H24" s="2">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="I24" s="3"/>
+      <c r="J24" s="3"/>
+    </row>
+    <row r="25" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C25" s="2">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="H25" s="2">
+        <f t="shared" si="1"/>
+        <v>21</v>
+      </c>
+      <c r="I25" s="3"/>
+      <c r="J25" s="3"/>
+    </row>
+    <row r="26" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C26" s="2">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="H26" s="2">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+      <c r="I26" s="3"/>
+      <c r="J26" s="3"/>
+    </row>
+    <row r="27" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C27" s="2">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="H27" s="2">
+        <f t="shared" si="1"/>
+        <v>23</v>
+      </c>
+      <c r="I27" s="3"/>
+      <c r="J27" s="3"/>
+    </row>
+    <row r="28" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C28" s="2">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="H28" s="2">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="I28" s="3"/>
+      <c r="J28" s="3"/>
+    </row>
+    <row r="29" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C29" s="2">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="H29" s="2">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="I29" s="3"/>
+      <c r="J29" s="3"/>
+    </row>
+    <row r="30" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C30" s="2">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="H30" s="2">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
+      <c r="I30" s="3"/>
+      <c r="J30" s="3"/>
+    </row>
+    <row r="31" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C31" s="2">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="H31" s="2">
+        <f t="shared" si="1"/>
+        <v>27</v>
+      </c>
+      <c r="I31" s="3"/>
+      <c r="J31" s="3"/>
+    </row>
+    <row r="32" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C32" s="2">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="H32" s="2">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
+      <c r="I32" s="3"/>
+      <c r="J32" s="3"/>
+    </row>
+    <row r="33" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C33" s="2">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="H33" s="2">
+        <f t="shared" si="1"/>
+        <v>29</v>
+      </c>
+      <c r="I33" s="3"/>
+      <c r="J33" s="3"/>
+    </row>
+    <row r="34" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C34" s="2">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+      <c r="H34" s="2">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="I34" s="3"/>
+      <c r="J34" s="3"/>
+    </row>
+    <row r="35" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C35" s="2">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
+      <c r="H35" s="2">
+        <f t="shared" si="1"/>
+        <v>31</v>
+      </c>
+      <c r="I35" s="3"/>
+      <c r="J35" s="3"/>
+    </row>
+    <row r="36" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C36" s="2">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="D36" s="3"/>
+      <c r="E36" s="3"/>
+      <c r="H36" s="2">
+        <f t="shared" si="1"/>
+        <v>32</v>
+      </c>
+      <c r="I36" s="3"/>
+      <c r="J36" s="3"/>
+    </row>
+    <row r="37" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C37" s="2">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="D37" s="3"/>
+      <c r="E37" s="3"/>
+      <c r="H37" s="2">
+        <f t="shared" si="1"/>
+        <v>33</v>
+      </c>
+      <c r="I37" s="3"/>
+      <c r="J37" s="3"/>
+    </row>
+    <row r="38" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C38" s="2">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="D38" s="3"/>
+      <c r="E38" s="3"/>
+      <c r="H38" s="2">
+        <f t="shared" si="1"/>
+        <v>34</v>
+      </c>
+      <c r="I38" s="3"/>
+      <c r="J38" s="3"/>
+    </row>
+    <row r="39" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C39" s="2">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="D39" s="3"/>
+      <c r="E39" s="3"/>
+      <c r="H39" s="2">
+        <f t="shared" si="1"/>
+        <v>35</v>
+      </c>
+      <c r="I39" s="3"/>
+      <c r="J39" s="3"/>
+    </row>
+    <row r="40" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C40" s="2">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="D40" s="3"/>
+      <c r="E40" s="3"/>
+      <c r="H40" s="2">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+      <c r="I40" s="3"/>
+      <c r="J40" s="3"/>
+    </row>
+    <row r="41" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C41" s="2">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="D41" s="3"/>
+      <c r="E41" s="3"/>
+      <c r="H41" s="2">
+        <f t="shared" si="1"/>
+        <v>37</v>
+      </c>
+      <c r="I41" s="3"/>
+      <c r="J41" s="3"/>
+    </row>
+    <row r="42" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C42" s="2">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="D42" s="3"/>
+      <c r="E42" s="3"/>
+      <c r="H42" s="2">
+        <f t="shared" si="1"/>
+        <v>38</v>
+      </c>
+      <c r="I42" s="3"/>
+      <c r="J42" s="3"/>
+    </row>
+    <row r="43" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C43" s="2">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="D43" s="3"/>
+      <c r="E43" s="3"/>
+      <c r="H43" s="2">
+        <f t="shared" si="1"/>
+        <v>39</v>
+      </c>
+      <c r="I43" s="3"/>
+      <c r="J43" s="3"/>
+    </row>
+    <row r="44" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C44" s="2">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="D44" s="3"/>
+      <c r="E44" s="3"/>
+      <c r="H44" s="2">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="I44" s="3"/>
+      <c r="J44" s="3"/>
+    </row>
+    <row r="45" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C45" s="2">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="D45" s="3"/>
+      <c r="E45" s="3"/>
+      <c r="H45" s="2">
+        <f t="shared" si="1"/>
+        <v>41</v>
+      </c>
+      <c r="I45" s="3"/>
+      <c r="J45" s="3"/>
+    </row>
+    <row r="46" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C46" s="2">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="D46" s="3"/>
+      <c r="E46" s="3"/>
+      <c r="H46" s="2">
+        <f t="shared" si="1"/>
+        <v>42</v>
+      </c>
+      <c r="I46" s="3"/>
+      <c r="J46" s="3"/>
+    </row>
+    <row r="47" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C47" s="2">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+      <c r="D47" s="3"/>
+      <c r="E47" s="3"/>
+      <c r="H47" s="2">
+        <f t="shared" si="1"/>
+        <v>43</v>
+      </c>
+      <c r="I47" s="3"/>
+      <c r="J47" s="3"/>
+    </row>
+    <row r="48" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C48" s="2">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+      <c r="D48" s="3"/>
+      <c r="E48" s="3"/>
+      <c r="H48" s="2">
+        <f t="shared" si="1"/>
+        <v>44</v>
+      </c>
+      <c r="I48" s="3"/>
+      <c r="J48" s="3"/>
+    </row>
+    <row r="49" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C49" s="2">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="D49" s="3"/>
+      <c r="E49" s="3"/>
+      <c r="H49" s="2">
+        <f t="shared" si="1"/>
+        <v>45</v>
+      </c>
+      <c r="I49" s="3"/>
+      <c r="J49" s="3"/>
+    </row>
+    <row r="50" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C50" s="2">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+      <c r="D50" s="3"/>
+      <c r="E50" s="3"/>
+      <c r="H50" s="2">
+        <f t="shared" si="1"/>
+        <v>46</v>
+      </c>
+      <c r="I50" s="3"/>
+      <c r="J50" s="3"/>
+    </row>
+    <row r="51" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C51" s="2">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="D51" s="3"/>
+      <c r="E51" s="3"/>
+      <c r="H51" s="2">
+        <f t="shared" si="1"/>
+        <v>47</v>
+      </c>
+      <c r="I51" s="3"/>
+      <c r="J51" s="3"/>
+    </row>
+    <row r="52" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C52" s="2">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+      <c r="D52" s="3"/>
+      <c r="E52" s="3"/>
+      <c r="H52" s="2">
+        <f t="shared" si="1"/>
+        <v>48</v>
+      </c>
+      <c r="I52" s="3"/>
+      <c r="J52" s="3"/>
+    </row>
+    <row r="53" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C53" s="2">
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
+      <c r="D53" s="3"/>
+      <c r="E53" s="3"/>
+      <c r="H53" s="2">
+        <f t="shared" si="1"/>
+        <v>49</v>
+      </c>
+      <c r="I53" s="3"/>
+      <c r="J53" s="3"/>
+    </row>
+    <row r="54" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C54" s="2">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="D54" s="3"/>
+      <c r="E54" s="3"/>
+      <c r="H54" s="2">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="I54" s="3"/>
+      <c r="J54" s="3"/>
+    </row>
+    <row r="56" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C56" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D56" s="3" t="e">
+        <f>AVERAGE(D5:D54)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E56" s="3" t="e">
+        <f>AVERAGE(E5:E54)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G56" s="3"/>
+      <c r="H56" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I56" s="3" t="e">
+        <f>AVERAGE(I5:I54)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J56" s="3" t="e">
+        <f>AVERAGE(J5:J54)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="57" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C57" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D57" s="3" t="e">
+        <f>_xlfn.STDEV.S(D5:D54)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E57" s="3" t="e">
+        <f>_xlfn.STDEV.S(E5:E54)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G57" s="3"/>
+      <c r="H57" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I57" s="3" t="e">
+        <f>_xlfn.STDEV.S(I5:I54)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J57" s="3" t="e">
+        <f>_xlfn.STDEV.S(J5:J54)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Test-2 and test-3 results
</commit_message>
<xml_diff>
--- a/migforecasting/underground/test-2.xlsx
+++ b/migforecasting/underground/test-2.xlsx
@@ -1421,8 +1421,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:T59"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:J57"/>
+    <sheetView topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="L72" sqref="L72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3117,7 +3117,7 @@
   <dimension ref="C3:J57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+      <selection activeCell="N52" sqref="N52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3158,751 +3158,1152 @@
       <c r="C5" s="2">
         <v>1</v>
       </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
+      <c r="D5" s="3">
+        <v>1.325146370336421</v>
+      </c>
+      <c r="E5" s="3">
+        <v>2.244994457539343</v>
+      </c>
       <c r="H5" s="2">
         <v>1</v>
       </c>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
+      <c r="I5" s="3">
+        <v>1.05545463115041</v>
+      </c>
+      <c r="J5" s="3">
+        <v>1.84341429581439</v>
+      </c>
     </row>
     <row r="6" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C6" s="2">
         <f>C5+1</f>
         <v>2</v>
       </c>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
+      <c r="D6" s="3">
+        <v>1.18167410699869</v>
+      </c>
+      <c r="E6" s="3">
+        <v>1.9922388707516161</v>
+      </c>
       <c r="H6" s="2">
         <f>H5+1</f>
         <v>2</v>
       </c>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
+      <c r="I6" s="3">
+        <v>1.130145906523321</v>
+      </c>
+      <c r="J6" s="3">
+        <v>2.2241746942377811</v>
+      </c>
     </row>
     <row r="7" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C7" s="2">
         <f t="shared" ref="C7:C54" si="0">C6+1</f>
         <v>3</v>
       </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
+      <c r="D7" s="3">
+        <v>1.012410263939284</v>
+      </c>
+      <c r="E7" s="3">
+        <v>2.617453228847503</v>
+      </c>
       <c r="H7" s="2">
         <f t="shared" ref="H7:H54" si="1">H6+1</f>
         <v>3</v>
       </c>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
+      <c r="I7" s="3">
+        <v>1.025296884987877</v>
+      </c>
+      <c r="J7" s="3">
+        <v>2.470617795752446</v>
+      </c>
     </row>
     <row r="8" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C8" s="2">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
+      <c r="D8" s="3">
+        <v>1.170823023880053</v>
+      </c>
+      <c r="E8" s="3">
+        <v>2.6874629171434532</v>
+      </c>
       <c r="H8" s="2">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
+      <c r="I8" s="3">
+        <v>1.094351739589376</v>
+      </c>
+      <c r="J8" s="3">
+        <v>1.878199761621411</v>
+      </c>
     </row>
     <row r="9" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C9" s="2">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
+      <c r="D9" s="3">
+        <v>1.1224242668853619</v>
+      </c>
+      <c r="E9" s="3">
+        <v>2.7084307440428832</v>
+      </c>
       <c r="H9" s="2">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
+      <c r="I9" s="3">
+        <v>1.22063926473162</v>
+      </c>
+      <c r="J9" s="3">
+        <v>3.267935696662529</v>
+      </c>
     </row>
     <row r="10" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C10" s="2">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
+      <c r="D10" s="3">
+        <v>1.2804999282459</v>
+      </c>
+      <c r="E10" s="3">
+        <v>2.9336812110623138</v>
+      </c>
       <c r="H10" s="2">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
+      <c r="I10" s="3">
+        <v>1.044825678279159</v>
+      </c>
+      <c r="J10" s="3">
+        <v>2.0944844448421569</v>
+      </c>
     </row>
     <row r="11" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C11" s="2">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
+      <c r="D11" s="3">
+        <v>1.1709781103784569</v>
+      </c>
+      <c r="E11" s="3">
+        <v>1.858538486428899</v>
+      </c>
       <c r="H11" s="2">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
+      <c r="I11" s="3">
+        <v>0.99717596954138699</v>
+      </c>
+      <c r="J11" s="3">
+        <v>3.301918392156781</v>
+      </c>
     </row>
     <row r="12" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C12" s="2">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
+      <c r="D12" s="3">
+        <v>1.153780341052558</v>
+      </c>
+      <c r="E12" s="3">
+        <v>3.067280617623712</v>
+      </c>
       <c r="H12" s="2">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
+      <c r="I12" s="3">
+        <v>0.99794616101968114</v>
+      </c>
+      <c r="J12" s="3">
+        <v>1.501272476593003</v>
+      </c>
     </row>
     <row r="13" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C13" s="2">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
+      <c r="D13" s="3">
+        <v>1.321833237066727</v>
+      </c>
+      <c r="E13" s="3">
+        <v>1.5396696637534419</v>
+      </c>
       <c r="H13" s="2">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
+      <c r="I13" s="3">
+        <v>1.256518634355176</v>
+      </c>
+      <c r="J13" s="3">
+        <v>1.4427478251052781</v>
+      </c>
     </row>
     <row r="14" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C14" s="2">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
+      <c r="D14" s="3">
+        <v>1.16981749779495</v>
+      </c>
+      <c r="E14" s="3">
+        <v>2.1234286648387042</v>
+      </c>
       <c r="H14" s="2">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
+      <c r="I14" s="3">
+        <v>1.0112294524721011</v>
+      </c>
+      <c r="J14" s="3">
+        <v>2.3805023486842272</v>
+      </c>
     </row>
     <row r="15" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C15" s="2">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
+      <c r="D15" s="3">
+        <v>1.1198020842833549</v>
+      </c>
+      <c r="E15" s="3">
+        <v>2.9087749020547702</v>
+      </c>
       <c r="H15" s="2">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="I15" s="3"/>
-      <c r="J15" s="3"/>
+      <c r="I15" s="3">
+        <v>0.97484203925445823</v>
+      </c>
+      <c r="J15" s="3">
+        <v>1.949313180891725</v>
+      </c>
     </row>
     <row r="16" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C16" s="2">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
+      <c r="D16" s="3">
+        <v>1.1319760322045489</v>
+      </c>
+      <c r="E16" s="3">
+        <v>2.7451151295516669</v>
+      </c>
       <c r="H16" s="2">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
+      <c r="I16" s="3">
+        <v>1.10607389945485</v>
+      </c>
+      <c r="J16" s="3">
+        <v>3.2681576485932649</v>
+      </c>
     </row>
     <row r="17" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C17" s="2">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
+      <c r="D17" s="3">
+        <v>1.0553509772419429</v>
+      </c>
+      <c r="E17" s="3">
+        <v>5.3454734558596888</v>
+      </c>
       <c r="H17" s="2">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
+      <c r="I17" s="3">
+        <v>1.0646280421143171</v>
+      </c>
+      <c r="J17" s="3">
+        <v>1.792612285500252</v>
+      </c>
     </row>
     <row r="18" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C18" s="2">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
+      <c r="D18" s="3">
+        <v>0.95832192078826905</v>
+      </c>
+      <c r="E18" s="3">
+        <v>6.719360924851248</v>
+      </c>
       <c r="H18" s="2">
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="I18" s="3"/>
-      <c r="J18" s="3"/>
+      <c r="I18" s="3">
+        <v>1.0198950655304639</v>
+      </c>
+      <c r="J18" s="3">
+        <v>2.9346367232374808</v>
+      </c>
     </row>
     <row r="19" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C19" s="2">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
+      <c r="D19" s="3">
+        <v>1.162305106697072</v>
+      </c>
+      <c r="E19" s="3">
+        <v>2.1846181447900781</v>
+      </c>
       <c r="H19" s="2">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="I19" s="3"/>
-      <c r="J19" s="3"/>
+      <c r="I19" s="3">
+        <v>0.89764219608081453</v>
+      </c>
+      <c r="J19" s="3">
+        <v>3.2887693776152358</v>
+      </c>
     </row>
     <row r="20" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C20" s="2">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
+      <c r="D20" s="3">
+        <v>1.3019158781407421</v>
+      </c>
+      <c r="E20" s="3">
+        <v>2.7104040081375991</v>
+      </c>
       <c r="H20" s="2">
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="I20" s="3"/>
-      <c r="J20" s="3"/>
+      <c r="I20" s="3">
+        <v>0.93456276775838476</v>
+      </c>
+      <c r="J20" s="3">
+        <v>1.2199909964125659</v>
+      </c>
     </row>
     <row r="21" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C21" s="2">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
+      <c r="D21" s="3">
+        <v>1.298540178388103</v>
+      </c>
+      <c r="E21" s="3">
+        <v>1.8946997433078661</v>
+      </c>
       <c r="H21" s="2">
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
-      <c r="I21" s="3"/>
-      <c r="J21" s="3"/>
+      <c r="I21" s="3">
+        <v>1.019413234045673</v>
+      </c>
+      <c r="J21" s="3">
+        <v>3.387335711752443</v>
+      </c>
     </row>
     <row r="22" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C22" s="2">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
+      <c r="D22" s="3">
+        <v>1.2335877040156209</v>
+      </c>
+      <c r="E22" s="3">
+        <v>2.1894171587306568</v>
+      </c>
       <c r="H22" s="2">
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
-      <c r="I22" s="3"/>
-      <c r="J22" s="3"/>
+      <c r="I22" s="3">
+        <v>1.065588681588248</v>
+      </c>
+      <c r="J22" s="3">
+        <v>1.429949095754377</v>
+      </c>
     </row>
     <row r="23" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C23" s="2">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
+      <c r="D23" s="3">
+        <v>0.99937874018810646</v>
+      </c>
+      <c r="E23" s="3">
+        <v>4.0913140849304952</v>
+      </c>
       <c r="H23" s="2">
         <f t="shared" si="1"/>
         <v>19</v>
       </c>
-      <c r="I23" s="3"/>
-      <c r="J23" s="3"/>
+      <c r="I23" s="3">
+        <v>1.012046594704624</v>
+      </c>
+      <c r="J23" s="3">
+        <v>2.1005027035766659</v>
+      </c>
     </row>
     <row r="24" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C24" s="2">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
+      <c r="D24" s="3">
+        <v>1.216745839907398</v>
+      </c>
+      <c r="E24" s="3">
+        <v>2.03411509754969</v>
+      </c>
       <c r="H24" s="2">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="I24" s="3"/>
-      <c r="J24" s="3"/>
+      <c r="I24" s="3">
+        <v>1.09734437311563</v>
+      </c>
+      <c r="J24" s="3">
+        <v>1.588036557655657</v>
+      </c>
     </row>
     <row r="25" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C25" s="2">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
+      <c r="D25" s="3">
+        <v>1.1998833635784449</v>
+      </c>
+      <c r="E25" s="3">
+        <v>1.997695865971362</v>
+      </c>
       <c r="H25" s="2">
         <f t="shared" si="1"/>
         <v>21</v>
       </c>
-      <c r="I25" s="3"/>
-      <c r="J25" s="3"/>
+      <c r="I25" s="3">
+        <v>0.87425362999341005</v>
+      </c>
+      <c r="J25" s="3">
+        <v>9.5852556743459232</v>
+      </c>
     </row>
     <row r="26" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C26" s="2">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
+      <c r="D26" s="3">
+        <v>0.94527749910955805</v>
+      </c>
+      <c r="E26" s="3">
+        <v>8.3704844084930006</v>
+      </c>
       <c r="H26" s="2">
         <f t="shared" si="1"/>
         <v>22</v>
       </c>
-      <c r="I26" s="3"/>
-      <c r="J26" s="3"/>
+      <c r="I26" s="3">
+        <v>0.96613195261154738</v>
+      </c>
+      <c r="J26" s="3">
+        <v>2.343128239023692</v>
+      </c>
     </row>
     <row r="27" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C27" s="2">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
+      <c r="D27" s="3">
+        <v>1.072823208544218</v>
+      </c>
+      <c r="E27" s="3">
+        <v>2.0842455664142649</v>
+      </c>
       <c r="H27" s="2">
         <f t="shared" si="1"/>
         <v>23</v>
       </c>
-      <c r="I27" s="3"/>
-      <c r="J27" s="3"/>
+      <c r="I27" s="3">
+        <v>0.99691540665785938</v>
+      </c>
+      <c r="J27" s="3">
+        <v>1.2174877153932431</v>
+      </c>
     </row>
     <row r="28" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C28" s="2">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
+      <c r="D28" s="3">
+        <v>1.109845356105001</v>
+      </c>
+      <c r="E28" s="3">
+        <v>2.1681520125931431</v>
+      </c>
       <c r="H28" s="2">
         <f t="shared" si="1"/>
         <v>24</v>
       </c>
-      <c r="I28" s="3"/>
-      <c r="J28" s="3"/>
+      <c r="I28" s="3">
+        <v>1.304079782706097</v>
+      </c>
+      <c r="J28" s="3">
+        <v>2.147522005372235</v>
+      </c>
     </row>
     <row r="29" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C29" s="2">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
+      <c r="D29" s="3">
+        <v>1.1338662000508519</v>
+      </c>
+      <c r="E29" s="3">
+        <v>2.2428713781384988</v>
+      </c>
       <c r="H29" s="2">
         <f t="shared" si="1"/>
         <v>25</v>
       </c>
-      <c r="I29" s="3"/>
-      <c r="J29" s="3"/>
+      <c r="I29" s="3">
+        <v>1.1812535930916019</v>
+      </c>
+      <c r="J29" s="3">
+        <v>2.3956054834596241</v>
+      </c>
     </row>
     <row r="30" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C30" s="2">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="D30" s="3"/>
-      <c r="E30" s="3"/>
+      <c r="D30" s="3">
+        <v>0.95443148299476843</v>
+      </c>
+      <c r="E30" s="3">
+        <v>7.427090410532192</v>
+      </c>
       <c r="H30" s="2">
         <f t="shared" si="1"/>
         <v>26</v>
       </c>
-      <c r="I30" s="3"/>
-      <c r="J30" s="3"/>
+      <c r="I30" s="3">
+        <v>1.0858151704242129</v>
+      </c>
+      <c r="J30" s="3">
+        <v>3.01552961488128</v>
+      </c>
     </row>
     <row r="31" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C31" s="2">
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-      <c r="D31" s="3"/>
-      <c r="E31" s="3"/>
+      <c r="D31" s="3">
+        <v>1.0807117326100351</v>
+      </c>
+      <c r="E31" s="3">
+        <v>2.478166178971835</v>
+      </c>
       <c r="H31" s="2">
         <f t="shared" si="1"/>
         <v>27</v>
       </c>
-      <c r="I31" s="3"/>
-      <c r="J31" s="3"/>
+      <c r="I31" s="3">
+        <v>1.090910108682245</v>
+      </c>
+      <c r="J31" s="3">
+        <v>2.1985904525004072</v>
+      </c>
     </row>
     <row r="32" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C32" s="2">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="D32" s="3"/>
-      <c r="E32" s="3"/>
+      <c r="D32" s="3">
+        <v>1.0599557294647479</v>
+      </c>
+      <c r="E32" s="3">
+        <v>2.07886994908226</v>
+      </c>
       <c r="H32" s="2">
         <f t="shared" si="1"/>
         <v>28</v>
       </c>
-      <c r="I32" s="3"/>
-      <c r="J32" s="3"/>
+      <c r="I32" s="3">
+        <v>0.96060074506323412</v>
+      </c>
+      <c r="J32" s="3">
+        <v>1.7569266899565541</v>
+      </c>
     </row>
     <row r="33" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C33" s="2">
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
-      <c r="D33" s="3"/>
-      <c r="E33" s="3"/>
+      <c r="D33" s="3">
+        <v>1.0212064659007969</v>
+      </c>
+      <c r="E33" s="3">
+        <v>3.5521985306726789</v>
+      </c>
       <c r="H33" s="2">
         <f t="shared" si="1"/>
         <v>29</v>
       </c>
-      <c r="I33" s="3"/>
-      <c r="J33" s="3"/>
+      <c r="I33" s="3">
+        <v>0.93966624451627767</v>
+      </c>
+      <c r="J33" s="3">
+        <v>5.3053484050788926</v>
+      </c>
     </row>
     <row r="34" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C34" s="2">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="D34" s="3"/>
-      <c r="E34" s="3"/>
+      <c r="D34" s="3">
+        <v>1.1294588802851739</v>
+      </c>
+      <c r="E34" s="3">
+        <v>1.6714516876576511</v>
+      </c>
       <c r="H34" s="2">
         <f t="shared" si="1"/>
         <v>30</v>
       </c>
-      <c r="I34" s="3"/>
-      <c r="J34" s="3"/>
+      <c r="I34" s="3">
+        <v>0.94247112485801521</v>
+      </c>
+      <c r="J34" s="3">
+        <v>2.7879567333765398</v>
+      </c>
     </row>
     <row r="35" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C35" s="2">
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
-      <c r="D35" s="3"/>
-      <c r="E35" s="3"/>
+      <c r="D35" s="3">
+        <v>1.169256064191587</v>
+      </c>
+      <c r="E35" s="3">
+        <v>1.910016306857238</v>
+      </c>
       <c r="H35" s="2">
         <f t="shared" si="1"/>
         <v>31</v>
       </c>
-      <c r="I35" s="3"/>
-      <c r="J35" s="3"/>
+      <c r="I35" s="3">
+        <v>1.103190761797354</v>
+      </c>
+      <c r="J35" s="3">
+        <v>1.1838434183499971</v>
+      </c>
     </row>
     <row r="36" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C36" s="2">
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
-      <c r="D36" s="3"/>
-      <c r="E36" s="3"/>
+      <c r="D36" s="3">
+        <v>1.135061845390718</v>
+      </c>
+      <c r="E36" s="3">
+        <v>3.0703409204245888</v>
+      </c>
       <c r="H36" s="2">
         <f t="shared" si="1"/>
         <v>32</v>
       </c>
-      <c r="I36" s="3"/>
-      <c r="J36" s="3"/>
+      <c r="I36" s="3">
+        <v>0.99599239418025631</v>
+      </c>
+      <c r="J36" s="3">
+        <v>2.6859106826049999</v>
+      </c>
     </row>
     <row r="37" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C37" s="2">
         <f t="shared" si="0"/>
         <v>33</v>
       </c>
-      <c r="D37" s="3"/>
-      <c r="E37" s="3"/>
+      <c r="D37" s="3">
+        <v>1.1429840902637709</v>
+      </c>
+      <c r="E37" s="3">
+        <v>2.119234569811681</v>
+      </c>
       <c r="H37" s="2">
         <f t="shared" si="1"/>
         <v>33</v>
       </c>
-      <c r="I37" s="3"/>
-      <c r="J37" s="3"/>
+      <c r="I37" s="3">
+        <v>0.88421772668703869</v>
+      </c>
+      <c r="J37" s="3">
+        <v>7.4571282772374268</v>
+      </c>
     </row>
     <row r="38" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C38" s="2">
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
-      <c r="D38" s="3"/>
-      <c r="E38" s="3"/>
+      <c r="D38" s="3">
+        <v>1.2215787155419471</v>
+      </c>
+      <c r="E38" s="3">
+        <v>1.9210254233659501</v>
+      </c>
       <c r="H38" s="2">
         <f t="shared" si="1"/>
         <v>34</v>
       </c>
-      <c r="I38" s="3"/>
-      <c r="J38" s="3"/>
+      <c r="I38" s="3">
+        <v>0.92282827622159436</v>
+      </c>
+      <c r="J38" s="3">
+        <v>2.3779252224130549</v>
+      </c>
     </row>
     <row r="39" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C39" s="2">
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
-      <c r="D39" s="3"/>
-      <c r="E39" s="3"/>
+      <c r="D39" s="3">
+        <v>1.0413789048502351</v>
+      </c>
+      <c r="E39" s="3">
+        <v>3.8039701791273699</v>
+      </c>
       <c r="H39" s="2">
         <f t="shared" si="1"/>
         <v>35</v>
       </c>
-      <c r="I39" s="3"/>
-      <c r="J39" s="3"/>
+      <c r="I39" s="3">
+        <v>0.95047600259877829</v>
+      </c>
+      <c r="J39" s="3">
+        <v>2.458899406641601</v>
+      </c>
     </row>
     <row r="40" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C40" s="2">
         <f t="shared" si="0"/>
         <v>36</v>
       </c>
-      <c r="D40" s="3"/>
-      <c r="E40" s="3"/>
+      <c r="D40" s="3">
+        <v>1.1280162102578599</v>
+      </c>
+      <c r="E40" s="3">
+        <v>2.1200652641245101</v>
+      </c>
       <c r="H40" s="2">
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
-      <c r="I40" s="3"/>
-      <c r="J40" s="3"/>
+      <c r="I40" s="3">
+        <v>1.002000689159479</v>
+      </c>
+      <c r="J40" s="3">
+        <v>1.675935665852389</v>
+      </c>
     </row>
     <row r="41" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C41" s="2">
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="D41" s="3"/>
-      <c r="E41" s="3"/>
+      <c r="D41" s="3">
+        <v>1.170412524002687</v>
+      </c>
+      <c r="E41" s="3">
+        <v>1.6613216268755799</v>
+      </c>
       <c r="H41" s="2">
         <f t="shared" si="1"/>
         <v>37</v>
       </c>
-      <c r="I41" s="3"/>
-      <c r="J41" s="3"/>
+      <c r="I41" s="3">
+        <v>0.93219599204192327</v>
+      </c>
+      <c r="J41" s="3">
+        <v>2.0647751520421069</v>
+      </c>
     </row>
     <row r="42" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C42" s="2">
         <f t="shared" si="0"/>
         <v>38</v>
       </c>
-      <c r="D42" s="3"/>
-      <c r="E42" s="3"/>
+      <c r="D42" s="3">
+        <v>1.058390073126418</v>
+      </c>
+      <c r="E42" s="3">
+        <v>5.180358852442791</v>
+      </c>
       <c r="H42" s="2">
         <f t="shared" si="1"/>
         <v>38</v>
       </c>
-      <c r="I42" s="3"/>
-      <c r="J42" s="3"/>
+      <c r="I42" s="3">
+        <v>1.0659004800310961</v>
+      </c>
+      <c r="J42" s="3">
+        <v>1.856222740618477</v>
+      </c>
     </row>
     <row r="43" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C43" s="2">
         <f t="shared" si="0"/>
         <v>39</v>
       </c>
-      <c r="D43" s="3"/>
-      <c r="E43" s="3"/>
+      <c r="D43" s="3">
+        <v>0.96780085952856676</v>
+      </c>
+      <c r="E43" s="3">
+        <v>9.3010580451319012</v>
+      </c>
       <c r="H43" s="2">
         <f t="shared" si="1"/>
         <v>39</v>
       </c>
-      <c r="I43" s="3"/>
-      <c r="J43" s="3"/>
+      <c r="I43" s="3">
+        <v>1.023673603105737</v>
+      </c>
+      <c r="J43" s="3">
+        <v>1.260114162244256</v>
+      </c>
     </row>
     <row r="44" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C44" s="2">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-      <c r="D44" s="3"/>
-      <c r="E44" s="3"/>
+      <c r="D44" s="3">
+        <v>1.086386857099406</v>
+      </c>
+      <c r="E44" s="3">
+        <v>3.441677926447023</v>
+      </c>
       <c r="H44" s="2">
         <f t="shared" si="1"/>
         <v>40</v>
       </c>
-      <c r="I44" s="3"/>
-      <c r="J44" s="3"/>
+      <c r="I44" s="3">
+        <v>0.99803056413907398</v>
+      </c>
+      <c r="J44" s="3">
+        <v>2.2841237282252922</v>
+      </c>
     </row>
     <row r="45" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C45" s="2">
         <f t="shared" si="0"/>
         <v>41</v>
       </c>
-      <c r="D45" s="3"/>
-      <c r="E45" s="3"/>
+      <c r="D45" s="3">
+        <v>0.94661481124806446</v>
+      </c>
+      <c r="E45" s="3">
+        <v>4.708003587954626</v>
+      </c>
       <c r="H45" s="2">
         <f t="shared" si="1"/>
         <v>41</v>
       </c>
-      <c r="I45" s="3"/>
-      <c r="J45" s="3"/>
+      <c r="I45" s="3">
+        <v>0.99771089494329901</v>
+      </c>
+      <c r="J45" s="3">
+        <v>1.3817508846450559</v>
+      </c>
     </row>
     <row r="46" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C46" s="2">
         <f t="shared" si="0"/>
         <v>42</v>
       </c>
-      <c r="D46" s="3"/>
-      <c r="E46" s="3"/>
+      <c r="D46" s="3">
+        <v>1.1718123928580511</v>
+      </c>
+      <c r="E46" s="3">
+        <v>1.6984693569958671</v>
+      </c>
       <c r="H46" s="2">
         <f t="shared" si="1"/>
         <v>42</v>
       </c>
-      <c r="I46" s="3"/>
-      <c r="J46" s="3"/>
+      <c r="I46" s="3">
+        <v>0.93862051168219762</v>
+      </c>
+      <c r="J46" s="3">
+        <v>1.3852038848668979</v>
+      </c>
     </row>
     <row r="47" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C47" s="2">
         <f t="shared" si="0"/>
         <v>43</v>
       </c>
-      <c r="D47" s="3"/>
-      <c r="E47" s="3"/>
+      <c r="D47" s="3">
+        <v>1.098077656137284</v>
+      </c>
+      <c r="E47" s="3">
+        <v>4.8520360374357363</v>
+      </c>
       <c r="H47" s="2">
         <f t="shared" si="1"/>
         <v>43</v>
       </c>
-      <c r="I47" s="3"/>
-      <c r="J47" s="3"/>
+      <c r="I47" s="3">
+        <v>0.99301037183785379</v>
+      </c>
+      <c r="J47" s="3">
+        <v>5.6109560852806801</v>
+      </c>
     </row>
     <row r="48" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C48" s="2">
         <f t="shared" si="0"/>
         <v>44</v>
       </c>
-      <c r="D48" s="3"/>
-      <c r="E48" s="3"/>
+      <c r="D48" s="3">
+        <v>1.0059205561646769</v>
+      </c>
+      <c r="E48" s="3">
+        <v>4.8710497560861876</v>
+      </c>
       <c r="H48" s="2">
         <f t="shared" si="1"/>
         <v>44</v>
       </c>
-      <c r="I48" s="3"/>
-      <c r="J48" s="3"/>
+      <c r="I48" s="3">
+        <v>1.018707654173016</v>
+      </c>
+      <c r="J48" s="3">
+        <v>4.2264641000687311</v>
+      </c>
     </row>
     <row r="49" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C49" s="2">
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
-      <c r="D49" s="3"/>
-      <c r="E49" s="3"/>
+      <c r="D49" s="3">
+        <v>1.210052135200578</v>
+      </c>
+      <c r="E49" s="3">
+        <v>2.0424784670193339</v>
+      </c>
       <c r="H49" s="2">
         <f t="shared" si="1"/>
         <v>45</v>
       </c>
-      <c r="I49" s="3"/>
-      <c r="J49" s="3"/>
+      <c r="I49" s="3">
+        <v>1.087094057367517</v>
+      </c>
+      <c r="J49" s="3">
+        <v>2.545943026627234</v>
+      </c>
     </row>
     <row r="50" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C50" s="2">
         <f t="shared" si="0"/>
         <v>46</v>
       </c>
-      <c r="D50" s="3"/>
-      <c r="E50" s="3"/>
+      <c r="D50" s="3">
+        <v>1.319256249443342</v>
+      </c>
+      <c r="E50" s="3">
+        <v>1.3511633710973749</v>
+      </c>
       <c r="H50" s="2">
         <f t="shared" si="1"/>
         <v>46</v>
       </c>
-      <c r="I50" s="3"/>
-      <c r="J50" s="3"/>
+      <c r="I50" s="3">
+        <v>0.94278088759596235</v>
+      </c>
+      <c r="J50" s="3">
+        <v>2.9151305539369252</v>
+      </c>
     </row>
     <row r="51" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C51" s="2">
         <f t="shared" si="0"/>
         <v>47</v>
       </c>
-      <c r="D51" s="3"/>
-      <c r="E51" s="3"/>
+      <c r="D51" s="3">
+        <v>1.19453037051095</v>
+      </c>
+      <c r="E51" s="3">
+        <v>2.812460373144837</v>
+      </c>
       <c r="H51" s="2">
         <f t="shared" si="1"/>
         <v>47</v>
       </c>
-      <c r="I51" s="3"/>
-      <c r="J51" s="3"/>
+      <c r="I51" s="3">
+        <v>1.1066800573108799</v>
+      </c>
+      <c r="J51" s="3">
+        <v>1.337752966364165</v>
+      </c>
     </row>
     <row r="52" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C52" s="2">
         <f t="shared" si="0"/>
         <v>48</v>
       </c>
-      <c r="D52" s="3"/>
-      <c r="E52" s="3"/>
+      <c r="D52" s="3">
+        <v>1.3230902950345691</v>
+      </c>
+      <c r="E52" s="3">
+        <v>3.1861822814312042</v>
+      </c>
       <c r="H52" s="2">
         <f t="shared" si="1"/>
         <v>48</v>
       </c>
-      <c r="I52" s="3"/>
-      <c r="J52" s="3"/>
+      <c r="I52" s="3">
+        <v>1.014048398586382</v>
+      </c>
+      <c r="J52" s="3">
+        <v>2.444823844915768</v>
+      </c>
     </row>
     <row r="53" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C53" s="2">
         <f t="shared" si="0"/>
         <v>49</v>
       </c>
-      <c r="D53" s="3"/>
-      <c r="E53" s="3"/>
+      <c r="D53" s="3">
+        <v>1.242665988905179</v>
+      </c>
+      <c r="E53" s="3">
+        <v>2.3692981904005568</v>
+      </c>
       <c r="H53" s="2">
         <f t="shared" si="1"/>
         <v>49</v>
       </c>
-      <c r="I53" s="3"/>
-      <c r="J53" s="3"/>
+      <c r="I53" s="3">
+        <v>1.208353056884574</v>
+      </c>
+      <c r="J53" s="3">
+        <v>1.5637250678978221</v>
+      </c>
     </row>
     <row r="54" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C54" s="2">
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
-      <c r="D54" s="3"/>
-      <c r="E54" s="3"/>
+      <c r="D54" s="3">
+        <v>1.1371430394724391</v>
+      </c>
+      <c r="E54" s="3">
+        <v>4.2520236242435256</v>
+      </c>
       <c r="H54" s="2">
         <f t="shared" si="1"/>
         <v>50</v>
       </c>
-      <c r="I54" s="3"/>
-      <c r="J54" s="3"/>
+      <c r="I54" s="3">
+        <v>1.054304862689724</v>
+      </c>
+      <c r="J54" s="3">
+        <v>2.295356237226708</v>
+      </c>
     </row>
     <row r="56" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C56" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D56" s="3" t="e">
+      <c r="D56" s="3">
         <f>AVERAGE(D5:D54)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E56" s="3" t="e">
+        <v>1.1373040233261094</v>
+      </c>
+      <c r="E56" s="3">
         <f>AVERAGE(E5:E54)</f>
-        <v>#DIV/0!</v>
+        <v>3.1467986332148081</v>
       </c>
       <c r="G56" s="3"/>
       <c r="H56" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="I56" s="3" t="e">
+      <c r="I56" s="3">
         <f>AVERAGE(I5:I54)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J56" s="3" t="e">
+        <v>1.0321507243587162</v>
+      </c>
+      <c r="J56" s="3">
         <f>AVERAGE(J5:J54)</f>
-        <v>#DIV/0!</v>
+        <v>2.5825981626781527</v>
       </c>
     </row>
     <row r="57" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C57" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D57" s="3" t="e">
+      <c r="D57" s="3">
         <f>_xlfn.STDEV.S(D5:D54)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E57" s="3" t="e">
+        <v>0.10500222986801089</v>
+      </c>
+      <c r="E57" s="3">
         <f>_xlfn.STDEV.S(E5:E54)</f>
-        <v>#DIV/0!</v>
+        <v>1.7621922733040305</v>
       </c>
       <c r="G57" s="3"/>
       <c r="H57" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="I57" s="3" t="e">
+      <c r="I57" s="3">
         <f>_xlfn.STDEV.S(I5:I54)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J57" s="3" t="e">
+        <v>9.2735273468703153E-2</v>
+      </c>
+      <c r="J57" s="3">
         <f>_xlfn.STDEV.S(J5:J54)</f>
-        <v>#DIV/0!</v>
+        <v>1.5553493939049186</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Test-2 (NN with MSE)
</commit_message>
<xml_diff>
--- a/migforecasting/underground/test-2.xlsx
+++ b/migforecasting/underground/test-2.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="18">
   <si>
     <t>train (MAPE)</t>
   </si>
@@ -68,6 +68,12 @@
   </si>
   <si>
     <t>Следующий год</t>
+  </si>
+  <si>
+    <t>test 20%</t>
+  </si>
+  <si>
+    <t>NN(64,64,64,64,1) (citiesdataset-NY-2.csv) - next year</t>
   </si>
 </sst>
 </file>
@@ -121,7 +127,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -135,6 +141,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -241,7 +250,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -362,7 +370,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -505,7 +512,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4138,10 +4144,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3:U65"/>
+  <dimension ref="C2:Z65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="T73" sqref="T73"/>
+    <sheetView tabSelected="1" topLeftCell="K22" workbookViewId="0">
+      <selection activeCell="X43" sqref="X43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4154,9 +4160,16 @@
     <col min="16" max="16" width="14.5703125" customWidth="1"/>
     <col min="20" max="20" width="13.85546875" customWidth="1"/>
     <col min="21" max="21" width="15.7109375" customWidth="1"/>
+    <col min="25" max="25" width="13" customWidth="1"/>
+    <col min="26" max="26" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="Y2" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C3" s="1" t="s">
         <v>10</v>
       </c>
@@ -4173,8 +4186,11 @@
         <v>11</v>
       </c>
       <c r="U3" s="1"/>
-    </row>
-    <row r="4" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="X3" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C4" s="2"/>
       <c r="D4" s="2" t="s">
         <v>0</v>
@@ -4203,8 +4219,14 @@
       <c r="U4" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="5" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="Y4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z4" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C5" s="2">
         <v>1</v>
       </c>
@@ -4241,8 +4263,17 @@
       <c r="U5" s="5">
         <v>5.2468442114396649E-3</v>
       </c>
-    </row>
-    <row r="6" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="X5" s="2">
+        <v>1</v>
+      </c>
+      <c r="Y5" s="5">
+        <v>9.2046183543042614E-4</v>
+      </c>
+      <c r="Z5" s="5">
+        <v>8.3932795195363705E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C6" s="2">
         <f>C5+1</f>
         <v>2</v>
@@ -4283,8 +4314,17 @@
       <c r="U6" s="5">
         <v>7.5675241412897047E-3</v>
       </c>
-    </row>
-    <row r="7" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="X6" s="2">
+        <v>2</v>
+      </c>
+      <c r="Y6" s="5">
+        <v>4.6212361669082508E-4</v>
+      </c>
+      <c r="Z6" s="5">
+        <v>7.6528724704759774E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C7" s="2">
         <f t="shared" ref="C7:C54" si="0">C6+1</f>
         <v>3</v>
@@ -4325,8 +4365,17 @@
       <c r="U7" s="5">
         <v>8.449671751109368E-3</v>
       </c>
-    </row>
-    <row r="8" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="X7" s="2">
+        <v>3</v>
+      </c>
+      <c r="Y7" s="5">
+        <v>7.490812499387127E-4</v>
+      </c>
+      <c r="Z7" s="5">
+        <v>1.124498069401093E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C8" s="2">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -4367,8 +4416,17 @@
       <c r="U8" s="5">
         <v>8.1514934583980011E-3</v>
       </c>
-    </row>
-    <row r="9" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="X8" s="2">
+        <v>4</v>
+      </c>
+      <c r="Y8" s="5">
+        <v>4.812933503987121E-4</v>
+      </c>
+      <c r="Z8" s="5">
+        <v>6.8430562474151987E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C9" s="2">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -4409,8 +4467,17 @@
       <c r="U9" s="5">
         <v>6.0148550817808871E-3</v>
       </c>
-    </row>
-    <row r="10" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="X9" s="2">
+        <v>5</v>
+      </c>
+      <c r="Y9" s="5">
+        <v>6.8160087661717043E-4</v>
+      </c>
+      <c r="Z9" s="5">
+        <v>6.8568495864527396E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C10" s="2">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -4451,8 +4518,17 @@
       <c r="U10" s="5">
         <v>8.0283505919435099E-3</v>
       </c>
-    </row>
-    <row r="11" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="X10" s="2">
+        <v>6</v>
+      </c>
+      <c r="Y10" s="5">
+        <v>1.014814980638644E-3</v>
+      </c>
+      <c r="Z10" s="5">
+        <v>1.117754553937866E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C11" s="2">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -4493,8 +4569,17 @@
       <c r="U11" s="5">
         <v>8.4415558465185704E-3</v>
       </c>
-    </row>
-    <row r="12" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="X11" s="2">
+        <v>7</v>
+      </c>
+      <c r="Y11" s="5">
+        <v>1.2268214597950171E-3</v>
+      </c>
+      <c r="Z11" s="5">
+        <v>7.4675544438988503E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C12" s="2">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -4535,8 +4620,17 @@
       <c r="U12" s="5">
         <v>1.071307152233464E-2</v>
       </c>
-    </row>
-    <row r="13" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="X12" s="2">
+        <v>8</v>
+      </c>
+      <c r="Y12" s="5">
+        <v>3.4457929102472891E-4</v>
+      </c>
+      <c r="Z12" s="5">
+        <v>6.6591300353251578E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C13" s="2">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -4577,8 +4671,17 @@
       <c r="U13" s="5">
         <v>6.7867135163552084E-3</v>
       </c>
-    </row>
-    <row r="14" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="X13" s="2">
+        <v>9</v>
+      </c>
+      <c r="Y13" s="5">
+        <v>6.1613838624861134E-4</v>
+      </c>
+      <c r="Z13" s="5">
+        <v>8.8318782515261658E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C14" s="2">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -4619,8 +4722,17 @@
       <c r="U14" s="5">
         <v>6.3120283448669517E-3</v>
       </c>
-    </row>
-    <row r="15" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="X14" s="2">
+        <v>10</v>
+      </c>
+      <c r="Y14" s="5">
+        <v>2.8212759633885408E-4</v>
+      </c>
+      <c r="Z14" s="5">
+        <v>1.256871074707251E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C15" s="2">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -4661,8 +4773,17 @@
       <c r="U15" s="5">
         <v>8.1151638031095961E-3</v>
       </c>
-    </row>
-    <row r="16" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="X15" s="2">
+        <v>11</v>
+      </c>
+      <c r="Y15" s="5">
+        <v>3.8192327472772489E-4</v>
+      </c>
+      <c r="Z15" s="5">
+        <v>7.2203541455874024E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C16" s="2">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -4703,8 +4824,17 @@
       <c r="U16" s="5">
         <v>7.135182705105673E-3</v>
       </c>
-    </row>
-    <row r="17" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="X16" s="2">
+        <v>12</v>
+      </c>
+      <c r="Y16" s="5">
+        <v>9.771344439018679E-4</v>
+      </c>
+      <c r="Z16" s="5">
+        <v>7.9873452337947438E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C17" s="2">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -4745,8 +4875,17 @@
       <c r="U17" s="5">
         <v>9.8232881176694552E-3</v>
       </c>
-    </row>
-    <row r="18" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="X17" s="2">
+        <v>13</v>
+      </c>
+      <c r="Y17" s="5">
+        <v>2.6288827336013411E-3</v>
+      </c>
+      <c r="Z17" s="5">
+        <v>7.0475122901448211E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C18" s="2">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -4787,8 +4926,17 @@
       <c r="U18" s="5">
         <v>9.3948872402644431E-3</v>
       </c>
-    </row>
-    <row r="19" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="X18" s="2">
+        <v>14</v>
+      </c>
+      <c r="Y18" s="5">
+        <v>5.4026527000035189E-4</v>
+      </c>
+      <c r="Z18" s="5">
+        <v>7.5757849929986828E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C19" s="2">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -4829,8 +4977,17 @@
       <c r="U19" s="5">
         <v>9.9604858809355188E-3</v>
       </c>
-    </row>
-    <row r="20" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="X19" s="2">
+        <v>15</v>
+      </c>
+      <c r="Y19" s="5">
+        <v>4.8317013864743533E-4</v>
+      </c>
+      <c r="Z19" s="5">
+        <v>1.0876356917816941E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C20" s="2">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -4871,8 +5028,17 @@
       <c r="U20" s="5">
         <v>8.634364418199111E-3</v>
       </c>
-    </row>
-    <row r="21" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="X20" s="2">
+        <v>16</v>
+      </c>
+      <c r="Y20" s="5">
+        <v>4.0908375660599658E-4</v>
+      </c>
+      <c r="Z20" s="5">
+        <v>9.4463593439375656E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C21" s="2">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -4913,8 +5079,17 @@
       <c r="U21" s="5">
         <v>6.9918872988264857E-3</v>
       </c>
-    </row>
-    <row r="22" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="X21" s="2">
+        <v>17</v>
+      </c>
+      <c r="Y21" s="5">
+        <v>3.0686784465563049E-4</v>
+      </c>
+      <c r="Z21" s="5">
+        <v>8.3865697230411877E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C22" s="2">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -4955,8 +5130,17 @@
       <c r="U22" s="5">
         <v>6.0674799029533932E-3</v>
       </c>
-    </row>
-    <row r="23" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="X22" s="2">
+        <v>18</v>
+      </c>
+      <c r="Y22" s="5">
+        <v>1.420066395684231E-3</v>
+      </c>
+      <c r="Z22" s="5">
+        <v>7.7057705457456611E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C23" s="2">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -4997,8 +5181,17 @@
       <c r="U23" s="5">
         <v>6.6286617613052464E-3</v>
       </c>
-    </row>
-    <row r="24" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="X23" s="2">
+        <v>19</v>
+      </c>
+      <c r="Y23" s="5">
+        <v>3.4848228971280963E-4</v>
+      </c>
+      <c r="Z23" s="5">
+        <v>8.3972866565599196E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C24" s="2">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -5039,8 +5232,17 @@
       <c r="U24" s="5">
         <v>8.1334055948972615E-3</v>
       </c>
-    </row>
-    <row r="25" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="X24" s="2">
+        <v>20</v>
+      </c>
+      <c r="Y24" s="5">
+        <v>5.6687513752917327E-4</v>
+      </c>
+      <c r="Z24" s="5">
+        <v>5.651943738905452E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C25" s="2">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -5081,8 +5283,11 @@
       <c r="U25" s="5">
         <v>8.7295106874431486E-3</v>
       </c>
-    </row>
-    <row r="26" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="X25" s="2"/>
+      <c r="Y25" s="5"/>
+      <c r="Z25" s="7"/>
+    </row>
+    <row r="26" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C26" s="2">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -5123,8 +5328,19 @@
       <c r="U26" s="5">
         <v>6.615170976816292E-3</v>
       </c>
-    </row>
-    <row r="27" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="X26" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y26" s="5">
+        <f>AVERAGE(Y5:Y24)</f>
+        <v>7.4208969640941324E-4</v>
+      </c>
+      <c r="Z26" s="5">
+        <f>AVERAGE(Z5:Z24)</f>
+        <v>8.3995570561812474E-3</v>
+      </c>
+    </row>
+    <row r="27" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C27" s="2">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -5165,8 +5381,19 @@
       <c r="U27" s="5">
         <v>6.3683103146324549E-3</v>
       </c>
-    </row>
-    <row r="28" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="X27" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="Y27" s="5">
+        <f>_xlfn.STDEV.S(Y5:Y24)</f>
+        <v>5.4652125350068378E-4</v>
+      </c>
+      <c r="Z27" s="5">
+        <f>_xlfn.STDEV.S(Z5:Z24)</f>
+        <v>1.8059641235904174E-3</v>
+      </c>
+    </row>
+    <row r="28" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C28" s="2">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -5207,8 +5434,10 @@
       <c r="U28" s="5">
         <v>8.4007810696122339E-3</v>
       </c>
-    </row>
-    <row r="29" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="Y28" s="7"/>
+      <c r="Z28" s="7"/>
+    </row>
+    <row r="29" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C29" s="2">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -5250,7 +5479,7 @@
         <v>6.9280999350673734E-3</v>
       </c>
     </row>
-    <row r="30" spans="3:21" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C30" s="2">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -5292,7 +5521,7 @@
         <v>6.2992242252402179E-3</v>
       </c>
     </row>
-    <row r="31" spans="3:21" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C31" s="2">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -5334,7 +5563,7 @@
         <v>5.9628344603574138E-3</v>
       </c>
     </row>
-    <row r="32" spans="3:21" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C32" s="2">
         <f t="shared" si="0"/>
         <v>28</v>

</xml_diff>